<commit_message>
Enhanced data dictionary documentation.
</commit_message>
<xml_diff>
--- a/data_dictionary_template.xlsx
+++ b/data_dictionary_template.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF2A031-ABCF-4B24-B20C-B7A0749544EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B454E7-A8D7-404C-A8A0-A4AF8052615B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{A411F62C-69E6-4132-9420-47BA5D60E3F5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A411F62C-69E6-4132-9420-47BA5D60E3F5}"/>
   </bookViews>
   <sheets>
     <sheet name="MOVIES_SCHEMA" sheetId="8" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="58">
   <si>
     <t>field_name</t>
   </si>
@@ -81,9 +81,6 @@
     <t>Float</t>
   </si>
   <si>
-    <t>UEI</t>
-  </si>
-  <si>
     <t>Boolean</t>
   </si>
   <si>
@@ -100,9 +97,6 @@
   </si>
   <si>
     <t>True/False to allow null values</t>
-  </si>
-  <si>
-    <t>Integer representing string max length</t>
   </si>
   <si>
     <t>Integer representing Min numerical value for a column</t>
@@ -132,9 +126,6 @@
   </si>
   <si>
     <t>required</t>
-  </si>
-  <si>
-    <t>Comments</t>
   </si>
   <si>
     <t>city</t>
@@ -929,12 +920,49 @@
       <t>$</t>
     </r>
   </si>
+  <si>
+    <t>Column or field name, case sensitive</t>
+  </si>
+  <si>
+    <t>Denotes when a column is required per schema</t>
+  </si>
+  <si>
+    <t>Denotes a primary key or unique value column/field</t>
+  </si>
+  <si>
+    <t>Integer representing string max length allowed</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Free text column for documenting additional column information.  This column is not used by the script and any additional columns will be ignored as well. </t>
+  </si>
+  <si>
+    <t>Optional</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Required Columns:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>All columns must be present for schema_vaildata to recognize sheets as schemas/ data dictionaries</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -958,13 +986,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1005,8 +1026,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="2" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="2" tint="-0.749992370372631"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1031,8 +1076,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -1055,78 +1106,339 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="2" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="2" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="2" tint="-0.499984740745262"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="2" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="2" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="2" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-0.499984740745262"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="2" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="2" tint="-0.499984740745262"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="2" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-0.499984740745262"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="2" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="2" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="2" tint="-0.499984740745262"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="2" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="2" tint="-0.499984740745262"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-0.499984740745262"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="2" tint="-0.499984740745262"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1140,9 +1452,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1180,7 +1492,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1286,7 +1598,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1428,7 +1740,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1436,11 +1748,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FE7144A-06F2-4903-AA7E-C1568298D9AA}">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K16" sqref="K16"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1458,355 +1770,266 @@
     <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:11" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="15" t="s">
+      <c r="B1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="J1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="15" t="s">
-        <v>32</v>
+      <c r="K1" s="9" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="16" t="s">
+      <c r="A2" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="17">
+      <c r="D2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="11">
         <v>7</v>
       </c>
-      <c r="F2" s="17">
+      <c r="F2" s="11">
         <v>1</v>
       </c>
-      <c r="G2" s="17">
+      <c r="G2" s="11">
         <v>9999999</v>
       </c>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16" t="s">
+      <c r="H2" s="10"/>
+      <c r="I2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="18"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="12"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="11">
+        <v>500</v>
+      </c>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11">
+        <v>1895</v>
+      </c>
+      <c r="G4" s="11">
+        <v>2025</v>
+      </c>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="11">
+        <v>500</v>
+      </c>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+    </row>
+    <row r="6" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C6" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="17">
+      <c r="D6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="11">
         <v>500</v>
       </c>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="K3" s="16"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="K6" s="10"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17">
-        <v>1895</v>
-      </c>
-      <c r="G4" s="17">
-        <v>2025</v>
-      </c>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4" s="16"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="D7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="11">
+        <v>3</v>
+      </c>
+      <c r="F7" s="11">
+        <v>1</v>
+      </c>
+      <c r="G7" s="11">
+        <v>5220</v>
+      </c>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="10"/>
+      <c r="K7" s="14"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B8" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="17">
-        <v>500</v>
-      </c>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="J5" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="K5" s="16"/>
-    </row>
-    <row r="6" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="16" t="s">
+      <c r="E8" s="11">
+        <v>2000</v>
+      </c>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="17">
-        <v>500</v>
-      </c>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="J6" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="K6" s="16"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" s="16" t="s">
+      <c r="C9" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="17">
-        <v>3</v>
-      </c>
-      <c r="F7" s="17">
-        <v>1</v>
-      </c>
-      <c r="G7" s="17">
-        <v>5220</v>
-      </c>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="J7" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="K7" s="20"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="17">
-        <v>2000</v>
-      </c>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="J8" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="K8" s="16"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="K9" s="16"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
     </row>
   </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E9" xr:uid="{5A3DB596-EC5A-4B35-9610-F2E4161CA6F7}">
+      <formula1>0</formula1>
+      <formula2>32767</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F9" xr:uid="{3476A79C-E820-4165-8730-79329A984A3B}">
+      <formula1>0</formula1>
+      <formula2>18446744073709500000</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G9" xr:uid="{D916072E-BB80-424D-A4AB-B1812C5081A7}">
+      <formula1>0</formula1>
+      <formula2>18446744073709500000</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
@@ -1844,11 +2067,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B509C83-C109-4026-9E95-FB776DC1CC9E}">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1867,378 +2090,265 @@
     <col min="12" max="12" width="30.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:11" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11">
+        <v>1</v>
+      </c>
+      <c r="G2" s="11">
+        <v>100000000</v>
+      </c>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="11">
+        <v>500</v>
+      </c>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="11">
+        <v>1000</v>
+      </c>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="11">
+        <v>500</v>
+      </c>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="15" t="s">
+      <c r="B6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="11">
         <v>2</v>
       </c>
-      <c r="E1" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="15" t="s">
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="K6" s="10"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="11">
         <v>5</v>
       </c>
-      <c r="H1" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="10"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" s="10"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16">
-        <v>1</v>
-      </c>
-      <c r="G2" s="16">
-        <v>100000000</v>
-      </c>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="16">
-        <v>500</v>
-      </c>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" s="16" t="s">
+      <c r="I9" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="16"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="16">
-        <v>1000</v>
-      </c>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4" s="16"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="16">
-        <v>500</v>
-      </c>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="J5" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="K5" s="16"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="16">
-        <v>2</v>
-      </c>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="J6" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="K6" s="16"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="16">
-        <v>5</v>
-      </c>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="I7" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="J7" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="K7" s="16"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="I8" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="J8" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="K8" s="16"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="I9" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="J9" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="K9" s="16"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
+      <c r="K9" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
+  <dataValidations count="2">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G9" xr:uid="{B66FD9AB-D84E-4B25-A66B-852D53BD5DB1}">
+      <formula1>0</formula1>
+      <formula2>18446744073709500000</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E9" xr:uid="{9355CEFC-A834-495B-97A3-FEFAEE42C1CB}">
+      <formula1>0</formula1>
+      <formula2>32767</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
@@ -2280,56 +2390,62 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="19.85546875" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" style="5" customWidth="1"/>
-    <col min="4" max="9" width="19.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="10" t="s">
+      <c r="B1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2337,13 +2453,13 @@
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="5" t="s">
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2361,7 +2477,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="2"/>
     </row>
@@ -2376,118 +2492,202 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1A441B5-D844-4857-B3E5-4EAD4026DBC2}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="50.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="30.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="39"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="23"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="23"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="18" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="C5" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="23"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="22">
+        <v>9</v>
+      </c>
+      <c r="D6" s="23"/>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="C7" s="22">
+        <v>0</v>
+      </c>
+      <c r="D7" s="23"/>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="5">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="C8" s="22">
+        <v>1000</v>
+      </c>
+      <c r="D8" s="23"/>
+    </row>
+    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="C9" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="5">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
+      <c r="D9" s="23"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="23"/>
+    </row>
+    <row r="11" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C11" s="32" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>28</v>
+      <c r="D11" s="24"/>
+    </row>
+    <row r="12" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="35"/>
+      <c r="D12" s="29" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D2:D11"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6152BEF2-804C-4668-AE10-B0EF9DB9B069}">
+          <x14:formula1>
+            <xm:f>Lists!$B$2:$B$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>C3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1FA26F47-E5CB-475E-8EE4-0DDC15988134}">
+          <x14:formula1>
+            <xm:f>Lists!$A$2:$A$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>C4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{09981679-A0E5-4400-A747-0848A203B103}">
+          <x14:formula1>
+            <xm:f>Lists!$C$2:$C$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>C5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5714B1A3-FA5C-443C-B998-785EB3BAC19A}">
+          <x14:formula1>
+            <xm:f>Lists!$H$2:$H$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>C10</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>